<commit_message>
excel updates, debug updates
</commit_message>
<xml_diff>
--- a/training/bak/Copy of results_9_28.xlsx
+++ b/training/bak/Copy of results_9_28.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\basill\research\steps\training\bak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B95557-27AA-4635-B46E-D0797165D916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F233CF-55DD-4955-B0D6-27E4718E4533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="4320" windowWidth="21600" windowHeight="11430"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_9_28" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="21">
   <si>
     <t>Subject</t>
   </si>
@@ -61,22 +72,37 @@
     <t>semiregular</t>
   </si>
   <si>
-    <t>AVG</t>
+    <t>Overall</t>
   </si>
   <si>
-    <t>AVG REG</t>
+    <t>Regular Gait</t>
   </si>
   <si>
-    <t>AVG IRR</t>
+    <t>Irregular Gait</t>
   </si>
   <si>
-    <t>AVG SEM</t>
+    <t>SemiRegular Gait</t>
+  </si>
+  <si>
+    <t>Wrist Sensor</t>
+  </si>
+  <si>
+    <t>Hip Sensor</t>
+  </si>
+  <si>
+    <t>Ankle Sensor</t>
+  </si>
+  <si>
+    <t>Average Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +419,30 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -569,9 +619,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -926,14 +996,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J275"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="L271" sqref="L271"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="L272" sqref="L272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -9608,55 +9683,105 @@
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H272" s="1" t="s">
+      <c r="H272" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I272" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J272" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="273" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H273" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I272" s="1">
+      <c r="I273" s="5">
         <f>AVERAGE(I$1:I$271)</f>
         <v>1.4652525925925926</v>
       </c>
-      <c r="J272" s="1">
+      <c r="J273" s="5">
         <f>AVERAGE(J$1:J$271)</f>
         <v>0.61781886121539076</v>
       </c>
     </row>
-    <row r="273" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H273" s="1" t="s">
+    <row r="274" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H274" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I273" s="1">
+      <c r="I274" s="6">
         <f>AVERAGEIF($B$1:$B$271,"regular",I$1:I$271)</f>
         <v>0.86183888888888904</v>
       </c>
-      <c r="J273" s="1">
+      <c r="J274" s="6">
         <f>AVERAGEIF($B$1:$B$271,"regular",J$1:J$271)</f>
         <v>0.84488267122718053</v>
       </c>
     </row>
-    <row r="274" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H274" s="1" t="s">
+    <row r="275" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H275" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I274" s="1">
+      <c r="I275" s="6">
         <f>AVERAGEIF($B$1:$B$271,"irregular",I$1:I$271)</f>
         <v>2.5969555555555557</v>
       </c>
-      <c r="J274" s="1">
+      <c r="J275" s="6">
         <f>AVERAGEIF($B$1:$B$271,"irregular",J$1:J$271)</f>
         <v>0.22434321382944628</v>
       </c>
     </row>
-    <row r="275" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H275" s="1" t="s">
+    <row r="276" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H276" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I275" s="1">
+      <c r="I276" s="6">
         <f>AVERAGEIF($B$1:$B$271,"semiregular",I$1:I$271)</f>
         <v>0.93696333333333304</v>
       </c>
-      <c r="J275" s="1">
+      <c r="J276" s="6">
         <f>AVERAGEIF($B$1:$B$271,"semiregular",J$1:J$271)</f>
         <v>0.78423069858954686</v>
+      </c>
+    </row>
+    <row r="277" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H277" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I277" s="7">
+        <f>AVERAGEIF($C$1:$C$271,"1",I$1:I$271)</f>
+        <v>1.5342266666666664</v>
+      </c>
+      <c r="J277" s="7">
+        <f>AVERAGEIF($C$1:$C$271,"1",J$1:J$271)</f>
+        <v>0.66112019754946683</v>
+      </c>
+    </row>
+    <row r="278" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H278" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I278" s="7">
+        <f>AVERAGEIF($C$1:$C$271,"2",I$1:I$271)</f>
+        <v>1.3580444444444446</v>
+      </c>
+      <c r="J278" s="7">
+        <f>AVERAGEIF($C$1:$C$271,"2",J$1:J$271)</f>
+        <v>0.57630244800534114</v>
+      </c>
+    </row>
+    <row r="279" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H279" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I279" s="7">
+        <f>AVERAGEIF($C$1:$C$271,"3",I$1:I$271)</f>
+        <v>1.5034866666666669</v>
+      </c>
+      <c r="J279" s="7">
+        <f>AVERAGEIF($C$1:$C$271,"3",J$1:J$271)</f>
+        <v>0.6160339380913652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>